<commit_message>
Auto commit - 10291713
</commit_message>
<xml_diff>
--- a/IM/202510_Service_Count_Report.xlsx
+++ b/IM/202510_Service_Count_Report.xlsx
@@ -275,10 +275,10 @@
     <t>台北市士林區德行西路100號</t>
   </si>
   <si>
+    <t>PM抄表</t>
+  </si>
+  <si>
     <t>服務</t>
-  </si>
-  <si>
-    <t>PM抄表</t>
   </si>
   <si>
     <t>10:27:00</t>
@@ -2763,22 +2763,22 @@
 換下 8187000916</t>
   </si>
   <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>新北市板橋區重慶路245巷61號</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
     <t>15:45:00</t>
   </si>
   <si>
-    <t>THILF0D349</t>
-  </si>
-  <si>
-    <t>新北市板橋區重慶路245巷61號</t>
-  </si>
-  <si>
-    <t>板橋成都店</t>
+    <t>驅動修復測試正常，請門市觀察中</t>
   </si>
   <si>
     <t>PMQ4 L99</t>
-  </si>
-  <si>
-    <t>驅動修復測試正常，請門市觀察中</t>
   </si>
   <si>
     <t>TX30000054</t>
@@ -3877,7 +3877,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>2025102727</v>
+        <v>2025102728</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3">
@@ -3923,9 +3923,7 @@
       <c r="R10" s="3">
         <v>2018</v>
       </c>
-      <c r="S10" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
@@ -3933,7 +3931,7 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA10" s="3" t="s">
         <v>40</v>
@@ -3947,7 +3945,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>2025102728</v>
+        <v>2025102727</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
@@ -3984,7 +3982,7 @@
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="7">
@@ -3993,7 +3991,9 @@
       <c r="R11" s="7">
         <v>2018</v>
       </c>
-      <c r="S11" s="7"/>
+      <c r="S11" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
@@ -4001,7 +4001,7 @@
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA11" s="7" t="s">
         <v>40</v>
@@ -4122,7 +4122,7 @@
         <v>94</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P13" s="7"/>
       <c r="Q13" s="7">
@@ -4141,7 +4141,7 @@
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA13" s="7" t="s">
         <v>40</v>
@@ -4211,7 +4211,7 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA14" s="3" t="s">
         <v>40</v>
@@ -4330,7 +4330,7 @@
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3">
@@ -4349,7 +4349,7 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>40</v>
@@ -4417,7 +4417,7 @@
       <c r="X17" s="7"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA17" s="7" t="s">
         <v>40</v>
@@ -4429,7 +4429,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>2025101693</v>
+        <v>2025101694</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -4468,7 +4468,7 @@
         <v>108</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3">
@@ -4477,9 +4477,7 @@
       <c r="R18" s="3">
         <v>2479</v>
       </c>
-      <c r="S18" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -4487,7 +4485,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA18" s="3" t="s">
         <v>40</v>
@@ -4501,7 +4499,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="7">
-        <v>2025101694</v>
+        <v>2025101693</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
@@ -4540,7 +4538,7 @@
         <v>108</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="7">
@@ -4549,7 +4547,9 @@
       <c r="R19" s="7">
         <v>2479</v>
       </c>
-      <c r="S19" s="7"/>
+      <c r="S19" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
@@ -4557,7 +4557,7 @@
       <c r="X19" s="7"/>
       <c r="Y19" s="7"/>
       <c r="Z19" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA19" s="7" t="s">
         <v>40</v>
@@ -4608,7 +4608,7 @@
         <v>108</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3">
@@ -4627,7 +4627,7 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA20" s="3" t="s">
         <v>40</v>
@@ -4697,7 +4697,7 @@
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
       <c r="Z21" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA21" s="7" t="s">
         <v>40</v>
@@ -4748,7 +4748,7 @@
         <v>52</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3">
@@ -4767,7 +4767,7 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA22" s="3" t="s">
         <v>40</v>
@@ -4837,7 +4837,7 @@
       <c r="X23" s="7"/>
       <c r="Y23" s="7"/>
       <c r="Z23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA23" s="7" t="s">
         <v>40</v>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -4977,7 +4977,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3">
-        <v>2025101688</v>
+        <v>2025101689</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -5016,16 +5016,14 @@
         <v>128</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3">
         <v>1845</v>
       </c>
-      <c r="S26" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -5033,7 +5031,7 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA26" s="3" t="s">
         <v>40</v>
@@ -5047,7 +5045,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="7">
-        <v>2025101689</v>
+        <v>2025101688</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
@@ -5086,14 +5084,16 @@
         <v>128</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="7">
         <v>1845</v>
       </c>
-      <c r="S27" s="7"/>
+      <c r="S27" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
@@ -5101,7 +5101,7 @@
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA27" s="7" t="s">
         <v>40</v>
@@ -5218,7 +5218,7 @@
         <v>30</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -5235,7 +5235,7 @@
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
@@ -5299,7 +5299,7 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA30" s="3" t="s">
         <v>40</v>
@@ -5350,7 +5350,7 @@
         <v>30</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
@@ -5418,7 +5418,7 @@
         <v>30</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
@@ -5435,7 +5435,7 @@
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA32" s="3" t="s">
         <v>40</v>
@@ -5503,7 +5503,7 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA33" s="7" t="s">
         <v>40</v>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="N34" s="6"/>
       <c r="O34" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
@@ -5680,7 +5680,7 @@
       </c>
       <c r="N36" s="6"/>
       <c r="O36" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
@@ -5750,7 +5750,7 @@
         <v>159</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
@@ -5767,7 +5767,7 @@
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
       <c r="Z37" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA37" s="7" t="s">
         <v>40</v>
@@ -5835,7 +5835,7 @@
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA38" s="3" t="s">
         <v>40</v>
@@ -5847,7 +5847,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7">
-        <v>2025102577</v>
+        <v>2025102578</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
@@ -5886,16 +5886,14 @@
         <v>30</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <v>36832</v>
       </c>
-      <c r="S39" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S39" s="7"/>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
@@ -5903,17 +5901,21 @@
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
       <c r="Z39" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA39" s="7"/>
-      <c r="AB39" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="AA39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB39" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:28">
       <c r="A40" s="3">
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2025102578</v>
+        <v>2025102577</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -5952,14 +5954,16 @@
         <v>30</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3">
         <v>36832</v>
       </c>
-      <c r="S40" s="3"/>
+      <c r="S40" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -5967,11 +5971,9 @@
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA40" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28">
@@ -6018,7 +6020,7 @@
         <v>169</v>
       </c>
       <c r="O41" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
@@ -6035,7 +6037,7 @@
       <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
       <c r="Z41" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA41" s="7" t="s">
         <v>40</v>
@@ -6103,7 +6105,7 @@
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA42" s="3" t="s">
         <v>40</v>
@@ -6152,7 +6154,7 @@
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
@@ -6169,7 +6171,7 @@
       <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
       <c r="Z43" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA43" s="7" t="s">
         <v>40</v>
@@ -6235,7 +6237,7 @@
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
       <c r="Z44" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA44" s="3" t="s">
         <v>40</v>
@@ -6284,7 +6286,7 @@
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
@@ -6354,7 +6356,7 @@
         <v>180</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
@@ -6371,7 +6373,7 @@
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA46" s="3" t="s">
         <v>40</v>
@@ -6439,7 +6441,7 @@
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
       <c r="Z47" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA47" s="7" t="s">
         <v>40</v>
@@ -6490,7 +6492,7 @@
         <v>30</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
@@ -6507,7 +6509,7 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
@@ -6571,7 +6573,7 @@
       <c r="X49" s="7"/>
       <c r="Y49" s="7"/>
       <c r="Z49" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA49" s="7" t="s">
         <v>40</v>
@@ -6622,7 +6624,7 @@
         <v>191</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P50" s="3"/>
       <c r="Q50" s="3">
@@ -6694,7 +6696,7 @@
         <v>159</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P51" s="7"/>
       <c r="Q51" s="7">
@@ -6713,7 +6715,7 @@
       <c r="X51" s="7"/>
       <c r="Y51" s="7"/>
       <c r="Z51" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA51" s="7" t="s">
         <v>40</v>
@@ -6783,7 +6785,7 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA52" s="3" t="s">
         <v>40</v>
@@ -6834,7 +6836,7 @@
         <v>159</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P53" s="7"/>
       <c r="Q53" s="7">
@@ -6906,7 +6908,7 @@
         <v>206</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P54" s="3"/>
       <c r="Q54" s="3">
@@ -6925,7 +6927,7 @@
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA54" s="3" t="s">
         <v>40</v>
@@ -6995,7 +6997,7 @@
       <c r="X55" s="7"/>
       <c r="Y55" s="7"/>
       <c r="Z55" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA55" s="7" t="s">
         <v>40</v>
@@ -7184,7 +7186,7 @@
         <v>223</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P58" s="3"/>
       <c r="Q58" s="3">
@@ -7203,7 +7205,7 @@
       <c r="X58" s="3"/>
       <c r="Y58" s="3"/>
       <c r="Z58" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA58" s="3" t="s">
         <v>40</v>
@@ -7273,7 +7275,7 @@
       <c r="X59" s="7"/>
       <c r="Y59" s="7"/>
       <c r="Z59" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA59" s="7" t="s">
         <v>40</v>
@@ -7390,7 +7392,7 @@
       </c>
       <c r="N61" s="8"/>
       <c r="O61" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
@@ -7485,7 +7487,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="7">
-        <v>2025103003</v>
+        <v>2025103002</v>
       </c>
       <c r="C63" s="7">
         <v>1</v>
@@ -7524,14 +7526,16 @@
         <v>236</v>
       </c>
       <c r="O63" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
       <c r="R63" s="7">
         <v>142499</v>
       </c>
-      <c r="S63" s="7"/>
+      <c r="S63" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T63" s="7"/>
       <c r="U63" s="7"/>
       <c r="V63" s="7"/>
@@ -7539,7 +7543,7 @@
       <c r="X63" s="7"/>
       <c r="Y63" s="7"/>
       <c r="Z63" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA63" s="7" t="s">
         <v>40</v>
@@ -7553,7 +7557,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3">
-        <v>2025103002</v>
+        <v>2025103003</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
@@ -7592,16 +7596,14 @@
         <v>236</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3">
         <v>142499</v>
       </c>
-      <c r="S64" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S64" s="3"/>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
       <c r="V64" s="3"/>
@@ -7609,7 +7611,7 @@
       <c r="X64" s="3"/>
       <c r="Y64" s="3"/>
       <c r="Z64" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA64" s="3" t="s">
         <v>40</v>
@@ -7660,7 +7662,7 @@
         <v>240</v>
       </c>
       <c r="O65" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -7677,7 +7679,7 @@
       <c r="X65" s="7"/>
       <c r="Y65" s="7"/>
       <c r="Z65" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA65" s="7" t="s">
         <v>40</v>
@@ -7745,7 +7747,7 @@
       <c r="X66" s="3"/>
       <c r="Y66" s="3"/>
       <c r="Z66" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA66" s="3" t="s">
         <v>40</v>
@@ -7792,7 +7794,7 @@
         <v>247</v>
       </c>
       <c r="O67" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P67" s="7"/>
       <c r="Q67" s="7"/>
@@ -7858,7 +7860,7 @@
         <v>254</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
@@ -7924,7 +7926,7 @@
         <v>259</v>
       </c>
       <c r="O69" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="7"/>
@@ -8056,7 +8058,7 @@
         <v>268</v>
       </c>
       <c r="O71" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P71" s="7"/>
       <c r="Q71" s="7"/>
@@ -8122,7 +8124,7 @@
         <v>273</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
@@ -8188,7 +8190,7 @@
         <v>277</v>
       </c>
       <c r="O73" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P73" s="7"/>
       <c r="Q73" s="7"/>
@@ -8322,7 +8324,7 @@
         <v>286</v>
       </c>
       <c r="O75" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P75" s="7"/>
       <c r="Q75" s="7"/>
@@ -8388,7 +8390,7 @@
         <v>289</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
@@ -8454,7 +8456,7 @@
         <v>294</v>
       </c>
       <c r="O77" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P77" s="7"/>
       <c r="Q77" s="7"/>
@@ -8520,7 +8522,7 @@
         <v>297</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
@@ -8586,7 +8588,7 @@
         <v>297</v>
       </c>
       <c r="O79" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P79" s="7"/>
       <c r="Q79" s="7"/>
@@ -8720,7 +8722,7 @@
         <v>303</v>
       </c>
       <c r="O81" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P81" s="7"/>
       <c r="Q81" s="7"/>
@@ -8784,7 +8786,7 @@
         <v>311</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
@@ -8850,7 +8852,7 @@
         <v>316</v>
       </c>
       <c r="O83" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P83" s="7"/>
       <c r="Q83" s="7"/>
@@ -8916,7 +8918,7 @@
         <v>321</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
@@ -8982,7 +8984,7 @@
         <v>325</v>
       </c>
       <c r="O85" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P85" s="7"/>
       <c r="Q85" s="7"/>
@@ -9184,7 +9186,7 @@
         <v>343</v>
       </c>
       <c r="O88" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
@@ -9386,7 +9388,7 @@
         <v>352</v>
       </c>
       <c r="O91" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P91" s="7"/>
       <c r="Q91" s="7"/>
@@ -9790,7 +9792,7 @@
         <v>366</v>
       </c>
       <c r="O97" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P97" s="7"/>
       <c r="Q97" s="7"/>
@@ -9854,7 +9856,7 @@
         <v>374</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P98" s="3"/>
       <c r="Q98" s="3"/>
@@ -9920,7 +9922,7 @@
         <v>377</v>
       </c>
       <c r="O99" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P99" s="7"/>
       <c r="Q99" s="7"/>
@@ -9986,7 +9988,7 @@
         <v>381</v>
       </c>
       <c r="O100" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P100" s="3"/>
       <c r="Q100" s="3"/>
@@ -10120,7 +10122,7 @@
         <v>388</v>
       </c>
       <c r="O102" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P102" s="3"/>
       <c r="Q102" s="3"/>
@@ -10186,7 +10188,7 @@
         <v>391</v>
       </c>
       <c r="O103" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P103" s="7"/>
       <c r="Q103" s="7"/>
@@ -10252,7 +10254,7 @@
         <v>395</v>
       </c>
       <c r="O104" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
@@ -10318,7 +10320,7 @@
         <v>400</v>
       </c>
       <c r="O105" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P105" s="7"/>
       <c r="Q105" s="7"/>
@@ -10384,7 +10386,7 @@
         <v>404</v>
       </c>
       <c r="O106" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P106" s="3"/>
       <c r="Q106" s="3"/>
@@ -10450,7 +10452,7 @@
         <v>408</v>
       </c>
       <c r="O107" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P107" s="7"/>
       <c r="Q107" s="7"/>
@@ -10516,7 +10518,7 @@
         <v>412</v>
       </c>
       <c r="O108" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
@@ -10582,7 +10584,7 @@
         <v>417</v>
       </c>
       <c r="O109" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P109" s="7"/>
       <c r="Q109" s="7"/>
@@ -10648,7 +10650,7 @@
         <v>421</v>
       </c>
       <c r="O110" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P110" s="3"/>
       <c r="Q110" s="3"/>
@@ -10714,7 +10716,7 @@
         <v>424</v>
       </c>
       <c r="O111" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P111" s="7"/>
       <c r="Q111" s="7"/>
@@ -10848,7 +10850,7 @@
         <v>427</v>
       </c>
       <c r="O113" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P113" s="7"/>
       <c r="Q113" s="7"/>
@@ -10914,7 +10916,7 @@
         <v>433</v>
       </c>
       <c r="O114" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
@@ -10980,7 +10982,7 @@
         <v>437</v>
       </c>
       <c r="O115" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P115" s="7"/>
       <c r="Q115" s="7"/>
@@ -11046,7 +11048,7 @@
         <v>437</v>
       </c>
       <c r="O116" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P116" s="3"/>
       <c r="Q116" s="3"/>
@@ -11112,7 +11114,7 @@
         <v>441</v>
       </c>
       <c r="O117" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P117" s="7"/>
       <c r="Q117" s="7"/>
@@ -11178,7 +11180,7 @@
         <v>446</v>
       </c>
       <c r="O118" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P118" s="3"/>
       <c r="Q118" s="3"/>
@@ -11312,7 +11314,7 @@
         <v>446</v>
       </c>
       <c r="O120" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P120" s="3"/>
       <c r="Q120" s="3"/>
@@ -11378,7 +11380,7 @@
         <v>454</v>
       </c>
       <c r="O121" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P121" s="7"/>
       <c r="Q121" s="7"/>
@@ -11444,7 +11446,7 @@
         <v>458</v>
       </c>
       <c r="O122" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P122" s="3"/>
       <c r="Q122" s="3"/>
@@ -11510,7 +11512,7 @@
         <v>463</v>
       </c>
       <c r="O123" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P123" s="7"/>
       <c r="Q123" s="7"/>
@@ -11644,7 +11646,7 @@
         <v>466</v>
       </c>
       <c r="O125" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P125" s="7"/>
       <c r="Q125" s="7"/>
@@ -11710,7 +11712,7 @@
         <v>471</v>
       </c>
       <c r="O126" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
@@ -11776,7 +11778,7 @@
         <v>474</v>
       </c>
       <c r="O127" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P127" s="7"/>
       <c r="Q127" s="7"/>
@@ -11910,7 +11912,7 @@
         <v>480</v>
       </c>
       <c r="O129" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P129" s="7"/>
       <c r="Q129" s="7"/>
@@ -11974,7 +11976,7 @@
         <v>485</v>
       </c>
       <c r="O130" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P130" s="3"/>
       <c r="Q130" s="3"/>
@@ -12044,7 +12046,7 @@
         <v>491</v>
       </c>
       <c r="O131" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P131" s="7"/>
       <c r="Q131" s="7">
@@ -12184,7 +12186,7 @@
         <v>491</v>
       </c>
       <c r="O133" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P133" s="7"/>
       <c r="Q133" s="7">
@@ -12256,7 +12258,7 @@
         <v>499</v>
       </c>
       <c r="O134" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P134" s="3"/>
       <c r="Q134" s="3">
@@ -12390,7 +12392,7 @@
       </c>
       <c r="N136" s="6"/>
       <c r="O136" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P136" s="3"/>
       <c r="Q136" s="3">
@@ -12528,7 +12530,7 @@
         <v>507</v>
       </c>
       <c r="O138" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P138" s="3"/>
       <c r="Q138" s="3">
@@ -12600,7 +12602,7 @@
         <v>507</v>
       </c>
       <c r="O139" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P139" s="7"/>
       <c r="Q139" s="7">
@@ -12810,7 +12812,7 @@
         <v>514</v>
       </c>
       <c r="O142" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P142" s="3"/>
       <c r="Q142" s="3">
@@ -12946,7 +12948,7 @@
         <v>518</v>
       </c>
       <c r="O144" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P144" s="3"/>
       <c r="Q144" s="3">
@@ -13082,7 +13084,7 @@
         <v>521</v>
       </c>
       <c r="O146" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P146" s="3"/>
       <c r="Q146" s="3">
@@ -13154,7 +13156,7 @@
         <v>521</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P147" s="7"/>
       <c r="Q147" s="7">
@@ -13290,7 +13292,7 @@
         <v>525</v>
       </c>
       <c r="O149" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P149" s="7">
         <v>6677</v>
@@ -13434,7 +13436,7 @@
         <v>528</v>
       </c>
       <c r="O151" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P151" s="7">
         <v>1800</v>
@@ -13578,7 +13580,7 @@
         <v>532</v>
       </c>
       <c r="O153" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P153" s="7"/>
       <c r="Q153" s="7">
@@ -13718,7 +13720,7 @@
         <v>535</v>
       </c>
       <c r="O155" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P155" s="7">
         <v>117</v>
@@ -13862,7 +13864,7 @@
         <v>539</v>
       </c>
       <c r="O157" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P157" s="7"/>
       <c r="Q157" s="7">
@@ -14099,7 +14101,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="7">
-        <v>2025100085</v>
+        <v>2025100084</v>
       </c>
       <c r="C161" s="7">
         <v>1</v>
@@ -14138,7 +14140,7 @@
         <v>532</v>
       </c>
       <c r="O161" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P161" s="7"/>
       <c r="Q161" s="7">
@@ -14147,7 +14149,9 @@
       <c r="R161" s="7">
         <v>400</v>
       </c>
-      <c r="S161" s="7"/>
+      <c r="S161" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T161" s="7"/>
       <c r="U161" s="7"/>
       <c r="V161" s="7"/>
@@ -14169,7 +14173,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="3">
-        <v>2025100084</v>
+        <v>2025100085</v>
       </c>
       <c r="C162" s="3">
         <v>1</v>
@@ -14208,7 +14212,7 @@
         <v>532</v>
       </c>
       <c r="O162" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P162" s="3"/>
       <c r="Q162" s="3">
@@ -14217,9 +14221,7 @@
       <c r="R162" s="3">
         <v>400</v>
       </c>
-      <c r="S162" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S162" s="3"/>
       <c r="T162" s="3"/>
       <c r="U162" s="3"/>
       <c r="V162" s="3"/>
@@ -14348,7 +14350,7 @@
         <v>547</v>
       </c>
       <c r="O164" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P164" s="3"/>
       <c r="Q164" s="3">
@@ -14484,7 +14486,7 @@
         <v>547</v>
       </c>
       <c r="O166" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P166" s="3"/>
       <c r="Q166" s="3">
@@ -14556,7 +14558,7 @@
         <v>550</v>
       </c>
       <c r="O167" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P167" s="7"/>
       <c r="Q167" s="7">
@@ -14653,7 +14655,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="7">
-        <v>2025101233</v>
+        <v>2025101232</v>
       </c>
       <c r="C169" s="7">
         <v>1</v>
@@ -14692,7 +14694,7 @@
         <v>554</v>
       </c>
       <c r="O169" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P169" s="7"/>
       <c r="Q169" s="7">
@@ -14701,7 +14703,9 @@
       <c r="R169" s="7">
         <v>1179</v>
       </c>
-      <c r="S169" s="7"/>
+      <c r="S169" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T169" s="7"/>
       <c r="U169" s="7"/>
       <c r="V169" s="7"/>
@@ -14711,19 +14715,15 @@
       <c r="Z169" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="AA169" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB169" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA169" s="7"/>
+      <c r="AB169" s="7"/>
     </row>
     <row r="170" spans="1:28">
       <c r="A170" s="3">
         <v>168</v>
       </c>
       <c r="B170" s="3">
-        <v>2025101232</v>
+        <v>2025101233</v>
       </c>
       <c r="C170" s="3">
         <v>1</v>
@@ -14762,7 +14762,7 @@
         <v>554</v>
       </c>
       <c r="O170" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P170" s="3"/>
       <c r="Q170" s="3">
@@ -14771,9 +14771,7 @@
       <c r="R170" s="3">
         <v>1179</v>
       </c>
-      <c r="S170" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S170" s="3"/>
       <c r="T170" s="3"/>
       <c r="U170" s="3"/>
       <c r="V170" s="3"/>
@@ -14783,7 +14781,9 @@
       <c r="Z170" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AA170" s="3"/>
+      <c r="AA170" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AB170" s="3"/>
     </row>
     <row r="171" spans="1:28">
@@ -15170,7 +15170,7 @@
         <v>569</v>
       </c>
       <c r="O176" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P176" s="3"/>
       <c r="Q176" s="3"/>
@@ -15308,7 +15308,7 @@
         <v>578</v>
       </c>
       <c r="O178" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P178" s="3"/>
       <c r="Q178" s="3"/>
@@ -15442,7 +15442,7 @@
       </c>
       <c r="N180" s="6"/>
       <c r="O180" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P180" s="3"/>
       <c r="Q180" s="3"/>
@@ -15576,7 +15576,7 @@
         <v>585</v>
       </c>
       <c r="O182" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P182" s="3"/>
       <c r="Q182" s="3"/>
@@ -15712,7 +15712,7 @@
         <v>585</v>
       </c>
       <c r="O184" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P184" s="3"/>
       <c r="Q184" s="3"/>
@@ -15848,7 +15848,7 @@
         <v>590</v>
       </c>
       <c r="O186" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P186" s="3"/>
       <c r="Q186" s="3"/>
@@ -15980,7 +15980,7 @@
         <v>590</v>
       </c>
       <c r="O188" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P188" s="3"/>
       <c r="Q188" s="3"/>
@@ -16116,7 +16116,7 @@
         <v>595</v>
       </c>
       <c r="O190" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P190" s="3"/>
       <c r="Q190" s="3"/>
@@ -16213,7 +16213,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="3">
-        <v>2025100369</v>
+        <v>2025100368</v>
       </c>
       <c r="C192" s="3">
         <v>1</v>
@@ -16252,14 +16252,16 @@
         <v>599</v>
       </c>
       <c r="O192" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P192" s="3"/>
       <c r="Q192" s="3"/>
       <c r="R192" s="3">
         <v>155192</v>
       </c>
-      <c r="S192" s="3"/>
+      <c r="S192" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T192" s="3"/>
       <c r="U192" s="3"/>
       <c r="V192" s="3"/>
@@ -16281,7 +16283,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="7">
-        <v>2025100368</v>
+        <v>2025100369</v>
       </c>
       <c r="C193" s="7">
         <v>1</v>
@@ -16320,16 +16322,14 @@
         <v>599</v>
       </c>
       <c r="O193" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P193" s="7"/>
       <c r="Q193" s="7"/>
       <c r="R193" s="7">
         <v>155192</v>
       </c>
-      <c r="S193" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S193" s="7"/>
       <c r="T193" s="7"/>
       <c r="U193" s="7"/>
       <c r="V193" s="7"/>
@@ -16388,7 +16388,7 @@
         <v>602</v>
       </c>
       <c r="O194" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P194" s="3"/>
       <c r="Q194" s="3"/>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="N197" s="8"/>
       <c r="O197" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P197" s="7"/>
       <c r="Q197" s="7"/>
@@ -16722,7 +16722,7 @@
       </c>
       <c r="N199" s="8"/>
       <c r="O199" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P199" s="7"/>
       <c r="Q199" s="7"/>
@@ -16792,7 +16792,7 @@
         <v>565</v>
       </c>
       <c r="O200" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P200" s="3"/>
       <c r="Q200" s="3"/>
@@ -16862,7 +16862,7 @@
         <v>565</v>
       </c>
       <c r="O201" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P201" s="7"/>
       <c r="Q201" s="7"/>
@@ -16932,7 +16932,7 @@
         <v>613</v>
       </c>
       <c r="O202" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P202" s="3"/>
       <c r="Q202" s="3"/>
@@ -17064,7 +17064,7 @@
         <v>617</v>
       </c>
       <c r="O204" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P204" s="3"/>
       <c r="Q204" s="3"/>
@@ -17196,7 +17196,7 @@
         <v>620</v>
       </c>
       <c r="O206" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P206" s="3"/>
       <c r="Q206" s="3"/>
@@ -17328,7 +17328,7 @@
         <v>532</v>
       </c>
       <c r="O208" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P208" s="3"/>
       <c r="Q208" s="3"/>
@@ -17464,7 +17464,7 @@
         <v>625</v>
       </c>
       <c r="O210" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P210" s="3"/>
       <c r="Q210" s="3"/>
@@ -17600,7 +17600,7 @@
         <v>628</v>
       </c>
       <c r="O212" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P212" s="3"/>
       <c r="Q212" s="3"/>
@@ -17736,7 +17736,7 @@
         <v>631</v>
       </c>
       <c r="O214" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P214" s="3"/>
       <c r="Q214" s="3"/>
@@ -17833,7 +17833,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="3">
-        <v>2025100063</v>
+        <v>2025100064</v>
       </c>
       <c r="C216" s="3">
         <v>1</v>
@@ -17872,16 +17872,14 @@
         <v>634</v>
       </c>
       <c r="O216" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P216" s="3"/>
       <c r="Q216" s="3"/>
       <c r="R216" s="3">
         <v>2841</v>
       </c>
-      <c r="S216" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S216" s="3"/>
       <c r="T216" s="3"/>
       <c r="U216" s="3"/>
       <c r="V216" s="3"/>
@@ -17903,7 +17901,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="7">
-        <v>2025100064</v>
+        <v>2025100063</v>
       </c>
       <c r="C217" s="7">
         <v>1</v>
@@ -17942,14 +17940,16 @@
         <v>634</v>
       </c>
       <c r="O217" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P217" s="7"/>
       <c r="Q217" s="7"/>
       <c r="R217" s="7">
         <v>2841</v>
       </c>
-      <c r="S217" s="7"/>
+      <c r="S217" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T217" s="7"/>
       <c r="U217" s="7"/>
       <c r="V217" s="7"/>
@@ -18008,7 +18008,7 @@
         <v>547</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
@@ -18105,7 +18105,7 @@
         <v>218</v>
       </c>
       <c r="B220" s="3">
-        <v>2025102607</v>
+        <v>2025102606</v>
       </c>
       <c r="C220" s="3">
         <v>1</v>
@@ -18144,14 +18144,16 @@
         <v>634</v>
       </c>
       <c r="O220" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P220" s="3"/>
       <c r="Q220" s="3"/>
       <c r="R220" s="3">
         <v>1291</v>
       </c>
-      <c r="S220" s="3"/>
+      <c r="S220" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T220" s="3"/>
       <c r="U220" s="3"/>
       <c r="V220" s="3"/>
@@ -18161,19 +18163,15 @@
       <c r="Z220" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="AA220" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB220" s="3">
-        <v>1</v>
-      </c>
+      <c r="AA220" s="3"/>
+      <c r="AB220" s="3"/>
     </row>
     <row r="221" spans="1:28">
       <c r="A221" s="7">
         <v>219</v>
       </c>
       <c r="B221" s="7">
-        <v>2025102606</v>
+        <v>2025102607</v>
       </c>
       <c r="C221" s="7">
         <v>1</v>
@@ -18212,16 +18210,14 @@
         <v>634</v>
       </c>
       <c r="O221" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P221" s="7"/>
       <c r="Q221" s="7"/>
       <c r="R221" s="7">
         <v>1291</v>
       </c>
-      <c r="S221" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S221" s="7"/>
       <c r="T221" s="7"/>
       <c r="U221" s="7"/>
       <c r="V221" s="7"/>
@@ -18231,7 +18227,9 @@
       <c r="Z221" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="AA221" s="7"/>
+      <c r="AA221" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB221" s="7"/>
     </row>
     <row r="222" spans="1:28">
@@ -18278,7 +18276,7 @@
         <v>602</v>
       </c>
       <c r="O222" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P222" s="3"/>
       <c r="Q222" s="3"/>
@@ -18764,7 +18762,7 @@
         <v>653</v>
       </c>
       <c r="O229" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P229" s="7"/>
       <c r="Q229" s="7">
@@ -18900,7 +18898,7 @@
         <v>657</v>
       </c>
       <c r="O231" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P231" s="7"/>
       <c r="Q231" s="7">
@@ -18972,7 +18970,7 @@
         <v>657</v>
       </c>
       <c r="O232" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P232" s="3"/>
       <c r="Q232" s="3">
@@ -19044,7 +19042,7 @@
         <v>657</v>
       </c>
       <c r="O233" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P233" s="7"/>
       <c r="Q233" s="7">
@@ -19180,7 +19178,7 @@
         <v>634</v>
       </c>
       <c r="O235" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P235" s="7"/>
       <c r="Q235" s="7">
@@ -19316,7 +19314,7 @@
         <v>665</v>
       </c>
       <c r="O237" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P237" s="7"/>
       <c r="Q237" s="7"/>
@@ -19448,7 +19446,7 @@
         <v>668</v>
       </c>
       <c r="O239" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P239" s="7"/>
       <c r="Q239" s="7"/>
@@ -19580,7 +19578,7 @@
         <v>671</v>
       </c>
       <c r="O241" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P241" s="7"/>
       <c r="Q241" s="7"/>
@@ -19712,7 +19710,7 @@
         <v>674</v>
       </c>
       <c r="O243" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P243" s="7"/>
       <c r="Q243" s="7"/>
@@ -19848,7 +19846,7 @@
         <v>677</v>
       </c>
       <c r="O245" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P245" s="7"/>
       <c r="Q245" s="7"/>
@@ -19945,7 +19943,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="7">
-        <v>2025100505</v>
+        <v>2025100506</v>
       </c>
       <c r="C247" s="7">
         <v>1</v>
@@ -19984,16 +19982,14 @@
         <v>668</v>
       </c>
       <c r="O247" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P247" s="7"/>
       <c r="Q247" s="7"/>
       <c r="R247" s="7">
         <v>187561</v>
       </c>
-      <c r="S247" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S247" s="7"/>
       <c r="T247" s="7"/>
       <c r="U247" s="7"/>
       <c r="V247" s="7"/>
@@ -20003,15 +19999,19 @@
       <c r="Z247" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="AA247" s="7"/>
-      <c r="AB247" s="7"/>
+      <c r="AA247" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB247" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="248" spans="1:28">
       <c r="A248" s="3">
         <v>246</v>
       </c>
       <c r="B248" s="3">
-        <v>2025100506</v>
+        <v>2025100505</v>
       </c>
       <c r="C248" s="3">
         <v>1</v>
@@ -20050,14 +20050,16 @@
         <v>668</v>
       </c>
       <c r="O248" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P248" s="3"/>
       <c r="Q248" s="3"/>
       <c r="R248" s="3">
         <v>187561</v>
       </c>
-      <c r="S248" s="3"/>
+      <c r="S248" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T248" s="3"/>
       <c r="U248" s="3"/>
       <c r="V248" s="3"/>
@@ -20067,9 +20069,7 @@
       <c r="Z248" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AA248" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA248" s="3"/>
       <c r="AB248" s="3"/>
     </row>
     <row r="249" spans="1:28">
@@ -20116,7 +20116,7 @@
         <v>682</v>
       </c>
       <c r="O249" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P249" s="7"/>
       <c r="Q249" s="7"/>
@@ -20246,7 +20246,7 @@
       </c>
       <c r="N251" s="8"/>
       <c r="O251" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P251" s="7"/>
       <c r="Q251" s="7"/>
@@ -20378,7 +20378,7 @@
       </c>
       <c r="N253" s="8"/>
       <c r="O253" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P253" s="7"/>
       <c r="Q253" s="7"/>
@@ -20506,7 +20506,7 @@
       </c>
       <c r="N255" s="8"/>
       <c r="O255" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P255" s="7"/>
       <c r="Q255" s="7"/>
@@ -20607,7 +20607,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="7">
-        <v>2025100557</v>
+        <v>2025100558</v>
       </c>
       <c r="C257" s="7">
         <v>1</v>
@@ -20646,7 +20646,7 @@
         <v>532</v>
       </c>
       <c r="O257" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P257" s="7"/>
       <c r="Q257" s="7">
@@ -20655,9 +20655,7 @@
       <c r="R257" s="7">
         <v>8923</v>
       </c>
-      <c r="S257" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S257" s="7"/>
       <c r="T257" s="7"/>
       <c r="U257" s="7"/>
       <c r="V257" s="7"/>
@@ -20679,7 +20677,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="3">
-        <v>2025100558</v>
+        <v>2025100557</v>
       </c>
       <c r="C258" s="3">
         <v>1</v>
@@ -20718,7 +20716,7 @@
         <v>532</v>
       </c>
       <c r="O258" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P258" s="3"/>
       <c r="Q258" s="3">
@@ -20727,7 +20725,9 @@
       <c r="R258" s="3">
         <v>8923</v>
       </c>
-      <c r="S258" s="3"/>
+      <c r="S258" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T258" s="3"/>
       <c r="U258" s="3"/>
       <c r="V258" s="3"/>
@@ -20924,7 +20924,7 @@
         <v>590</v>
       </c>
       <c r="O261" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P261" s="7"/>
       <c r="Q261" s="7"/>
@@ -21124,7 +21124,7 @@
         <v>590</v>
       </c>
       <c r="O264" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P264" s="3"/>
       <c r="Q264" s="3"/>
@@ -21330,7 +21330,7 @@
         <v>715</v>
       </c>
       <c r="O267" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P267" s="7"/>
       <c r="Q267" s="7"/>
@@ -21429,7 +21429,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="7">
-        <v>2025100709</v>
+        <v>2025100708</v>
       </c>
       <c r="C269" s="7">
         <v>1</v>
@@ -21468,14 +21468,16 @@
         <v>718</v>
       </c>
       <c r="O269" s="7" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P269" s="7"/>
       <c r="Q269" s="7"/>
       <c r="R269" s="7">
         <v>28</v>
       </c>
-      <c r="S269" s="7"/>
+      <c r="S269" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T269" s="7"/>
       <c r="U269" s="7"/>
       <c r="V269" s="7"/>
@@ -21485,19 +21487,15 @@
       <c r="Z269" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="AA269" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB269" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA269" s="7"/>
+      <c r="AB269" s="7"/>
     </row>
     <row r="270" spans="1:28">
       <c r="A270" s="3">
         <v>268</v>
       </c>
       <c r="B270" s="3">
-        <v>2025100708</v>
+        <v>2025100709</v>
       </c>
       <c r="C270" s="3">
         <v>1</v>
@@ -21536,16 +21534,14 @@
         <v>718</v>
       </c>
       <c r="O270" s="3" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P270" s="3"/>
       <c r="Q270" s="3"/>
       <c r="R270" s="3">
         <v>28</v>
       </c>
-      <c r="S270" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S270" s="3"/>
       <c r="T270" s="3"/>
       <c r="U270" s="3"/>
       <c r="V270" s="3"/>
@@ -21555,7 +21551,9 @@
       <c r="Z270" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AA270" s="3"/>
+      <c r="AA270" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AB270" s="3"/>
     </row>
     <row r="271" spans="1:28">
@@ -21602,7 +21600,7 @@
         <v>671</v>
       </c>
       <c r="O271" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P271" s="7"/>
       <c r="Q271" s="7"/>
@@ -21734,7 +21732,7 @@
         <v>723</v>
       </c>
       <c r="O273" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P273" s="7"/>
       <c r="Q273" s="7"/>
@@ -21872,7 +21870,7 @@
         <v>668</v>
       </c>
       <c r="O275" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P275" s="7"/>
       <c r="Q275" s="7">
@@ -22080,7 +22078,7 @@
         <v>693</v>
       </c>
       <c r="O278" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P278" s="3"/>
       <c r="Q278" s="3"/>
@@ -22152,7 +22150,7 @@
         <v>693</v>
       </c>
       <c r="O279" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P279" s="7"/>
       <c r="Q279" s="7"/>
@@ -22222,7 +22220,7 @@
         <v>693</v>
       </c>
       <c r="O280" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P280" s="3"/>
       <c r="Q280" s="3"/>
@@ -22290,7 +22288,7 @@
         <v>737</v>
       </c>
       <c r="O281" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P281" s="7"/>
       <c r="Q281" s="7"/>
@@ -22360,7 +22358,7 @@
         <v>737</v>
       </c>
       <c r="O282" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P282" s="3"/>
       <c r="Q282" s="3"/>
@@ -22430,7 +22428,7 @@
         <v>737</v>
       </c>
       <c r="O283" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P283" s="7"/>
       <c r="Q283" s="7"/>
@@ -22500,7 +22498,7 @@
         <v>739</v>
       </c>
       <c r="O284" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P284" s="3"/>
       <c r="Q284" s="3"/>
@@ -22570,7 +22568,7 @@
         <v>739</v>
       </c>
       <c r="O285" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P285" s="7"/>
       <c r="Q285" s="7"/>
@@ -22640,7 +22638,7 @@
         <v>739</v>
       </c>
       <c r="O286" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P286" s="3"/>
       <c r="Q286" s="3"/>
@@ -22710,7 +22708,7 @@
         <v>602</v>
       </c>
       <c r="O287" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P287" s="7"/>
       <c r="Q287" s="7"/>
@@ -22807,7 +22805,7 @@
         <v>287</v>
       </c>
       <c r="B289" s="7">
-        <v>2025100079</v>
+        <v>2025100080</v>
       </c>
       <c r="C289" s="7">
         <v>1</v>
@@ -22846,16 +22844,14 @@
         <v>744</v>
       </c>
       <c r="O289" s="7" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="P289" s="7"/>
       <c r="Q289" s="7"/>
       <c r="R289" s="7">
         <v>68795</v>
       </c>
-      <c r="S289" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S289" s="7"/>
       <c r="T289" s="7"/>
       <c r="U289" s="7"/>
       <c r="V289" s="7"/>
@@ -22865,15 +22861,19 @@
       <c r="Z289" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="AA289" s="7"/>
-      <c r="AB289" s="7"/>
+      <c r="AA289" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB289" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="290" spans="1:28">
       <c r="A290" s="3">
         <v>288</v>
       </c>
       <c r="B290" s="3">
-        <v>2025100080</v>
+        <v>2025100079</v>
       </c>
       <c r="C290" s="3">
         <v>1</v>
@@ -22912,14 +22912,16 @@
         <v>744</v>
       </c>
       <c r="O290" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="P290" s="3"/>
       <c r="Q290" s="3"/>
       <c r="R290" s="3">
         <v>68795</v>
       </c>
-      <c r="S290" s="3"/>
+      <c r="S290" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T290" s="3"/>
       <c r="U290" s="3"/>
       <c r="V290" s="3"/>
@@ -22929,9 +22931,7 @@
       <c r="Z290" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AA290" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA290" s="3"/>
       <c r="AB290" s="3"/>
     </row>
     <row r="291" spans="1:28">
@@ -22978,7 +22978,7 @@
         <v>744</v>
       </c>
       <c r="O291" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P291" s="7"/>
       <c r="Q291" s="7"/>
@@ -23048,7 +23048,7 @@
         <v>746</v>
       </c>
       <c r="O292" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P292" s="3"/>
       <c r="Q292" s="3"/>
@@ -23118,7 +23118,7 @@
         <v>746</v>
       </c>
       <c r="O293" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P293" s="7"/>
       <c r="Q293" s="7"/>
@@ -23188,7 +23188,7 @@
         <v>746</v>
       </c>
       <c r="O294" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P294" s="3"/>
       <c r="Q294" s="3"/>
@@ -23258,7 +23258,7 @@
         <v>751</v>
       </c>
       <c r="O295" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P295" s="7"/>
       <c r="Q295" s="7">
@@ -23394,7 +23394,7 @@
         <v>751</v>
       </c>
       <c r="O297" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P297" s="7"/>
       <c r="Q297" s="7">
@@ -23466,7 +23466,7 @@
         <v>753</v>
       </c>
       <c r="O298" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P298" s="3"/>
       <c r="Q298" s="3">
@@ -23602,7 +23602,7 @@
         <v>753</v>
       </c>
       <c r="O300" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P300" s="3"/>
       <c r="Q300" s="3">
@@ -23670,7 +23670,7 @@
         <v>756</v>
       </c>
       <c r="O301" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P301" s="7"/>
       <c r="Q301" s="7"/>
@@ -23804,7 +23804,7 @@
         <v>759</v>
       </c>
       <c r="O303" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P303" s="7"/>
       <c r="Q303" s="7"/>
@@ -24004,7 +24004,7 @@
         <v>767</v>
       </c>
       <c r="O306" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P306" s="3"/>
       <c r="Q306" s="3"/>
@@ -24068,7 +24068,7 @@
         <v>771</v>
       </c>
       <c r="O307" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P307" s="7"/>
       <c r="Q307" s="7"/>
@@ -24270,7 +24270,7 @@
         <v>779</v>
       </c>
       <c r="O310" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P310" s="3"/>
       <c r="Q310" s="3"/>
@@ -24404,7 +24404,7 @@
         <v>782</v>
       </c>
       <c r="O312" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P312" s="3"/>
       <c r="Q312" s="3"/>
@@ -24670,7 +24670,7 @@
         <v>787</v>
       </c>
       <c r="O316" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P316" s="3"/>
       <c r="Q316" s="3"/>
@@ -24802,7 +24802,7 @@
         <v>792</v>
       </c>
       <c r="O318" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P318" s="3"/>
       <c r="Q318" s="3"/>
@@ -24934,7 +24934,7 @@
         <v>800</v>
       </c>
       <c r="O320" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P320" s="3"/>
       <c r="Q320" s="3"/>
@@ -25068,7 +25068,7 @@
         <v>804</v>
       </c>
       <c r="O322" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P322" s="3"/>
       <c r="Q322" s="3"/>
@@ -25202,7 +25202,7 @@
         <v>808</v>
       </c>
       <c r="O324" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P324" s="3"/>
       <c r="Q324" s="3"/>
@@ -25266,7 +25266,7 @@
         <v>812</v>
       </c>
       <c r="O325" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P325" s="7"/>
       <c r="Q325" s="7"/>
@@ -25334,7 +25334,7 @@
         <v>815</v>
       </c>
       <c r="O326" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P326" s="3"/>
       <c r="Q326" s="3"/>
@@ -25400,7 +25400,7 @@
         <v>815</v>
       </c>
       <c r="O327" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P327" s="7"/>
       <c r="Q327" s="7"/>
@@ -25530,7 +25530,7 @@
         <v>820</v>
       </c>
       <c r="O329" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P329" s="7"/>
       <c r="Q329" s="7"/>
@@ -25598,7 +25598,7 @@
         <v>823</v>
       </c>
       <c r="O330" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P330" s="3"/>
       <c r="Q330" s="3"/>
@@ -25664,7 +25664,7 @@
         <v>827</v>
       </c>
       <c r="O331" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P331" s="7"/>
       <c r="Q331" s="7"/>
@@ -25798,7 +25798,7 @@
         <v>830</v>
       </c>
       <c r="O333" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P333" s="7"/>
       <c r="Q333" s="7"/>
@@ -25932,7 +25932,7 @@
         <v>834</v>
       </c>
       <c r="O335" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P335" s="7"/>
       <c r="Q335" s="7"/>
@@ -26064,7 +26064,7 @@
         <v>840</v>
       </c>
       <c r="O337" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P337" s="7"/>
       <c r="Q337" s="7"/>
@@ -26406,7 +26406,7 @@
         <v>857</v>
       </c>
       <c r="O342" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P342" s="3"/>
       <c r="Q342" s="3"/>
@@ -26538,7 +26538,7 @@
         <v>860</v>
       </c>
       <c r="O344" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P344" s="3"/>
       <c r="Q344" s="3"/>
@@ -26670,7 +26670,7 @@
         <v>863</v>
       </c>
       <c r="O346" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P346" s="3"/>
       <c r="Q346" s="3"/>
@@ -26802,7 +26802,7 @@
         <v>869</v>
       </c>
       <c r="O348" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P348" s="3"/>
       <c r="Q348" s="3"/>
@@ -26872,7 +26872,7 @@
         <v>869</v>
       </c>
       <c r="O349" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P349" s="7"/>
       <c r="Q349" s="7"/>
@@ -27039,7 +27039,7 @@
         <v>350</v>
       </c>
       <c r="B352" s="3">
-        <v>2025102037</v>
+        <v>2025102005</v>
       </c>
       <c r="C352" s="3">
         <v>1</v>
@@ -27062,8 +27062,12 @@
       <c r="I352" s="3" t="s">
         <v>879</v>
       </c>
-      <c r="J352" s="3"/>
-      <c r="K352" s="3"/>
+      <c r="J352" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="K352" s="3" t="s">
+        <v>263</v>
+      </c>
       <c r="L352" s="6" t="s">
         <v>245</v>
       </c>
@@ -27074,16 +27078,14 @@
         <v>881</v>
       </c>
       <c r="O352" s="3" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="P352" s="3"/>
       <c r="Q352" s="3"/>
       <c r="R352" s="3">
         <v>0</v>
       </c>
-      <c r="S352" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S352" s="3"/>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
       <c r="V352" s="3"/>
@@ -27091,17 +27093,21 @@
       <c r="X352" s="3"/>
       <c r="Y352" s="3"/>
       <c r="Z352" s="6" t="s">
-        <v>816</v>
-      </c>
-      <c r="AA352" s="3"/>
-      <c r="AB352" s="3"/>
+        <v>882</v>
+      </c>
+      <c r="AA352" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB352" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="353" spans="1:28">
       <c r="A353" s="7">
         <v>351</v>
       </c>
       <c r="B353" s="7">
-        <v>2025102005</v>
+        <v>2025102037</v>
       </c>
       <c r="C353" s="7">
         <v>1</v>
@@ -27124,12 +27130,8 @@
       <c r="I353" s="7" t="s">
         <v>879</v>
       </c>
-      <c r="J353" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="K353" s="7" t="s">
-        <v>263</v>
-      </c>
+      <c r="J353" s="7"/>
+      <c r="K353" s="7"/>
       <c r="L353" s="8" t="s">
         <v>245</v>
       </c>
@@ -27140,14 +27142,16 @@
         <v>881</v>
       </c>
       <c r="O353" s="7" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="P353" s="7"/>
       <c r="Q353" s="7"/>
       <c r="R353" s="7">
         <v>0</v>
       </c>
-      <c r="S353" s="7"/>
+      <c r="S353" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T353" s="7"/>
       <c r="U353" s="7"/>
       <c r="V353" s="7"/>
@@ -27155,11 +27159,9 @@
       <c r="X353" s="7"/>
       <c r="Y353" s="7"/>
       <c r="Z353" s="8" t="s">
-        <v>882</v>
-      </c>
-      <c r="AA353" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>816</v>
+      </c>
+      <c r="AA353" s="7"/>
       <c r="AB353" s="7"/>
     </row>
     <row r="354" spans="1:28">
@@ -27202,7 +27204,7 @@
         <v>881</v>
       </c>
       <c r="O354" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P354" s="3"/>
       <c r="Q354" s="3"/>
@@ -27336,7 +27338,7 @@
         <v>894</v>
       </c>
       <c r="O356" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P356" s="3"/>
       <c r="Q356" s="3"/>
@@ -27497,7 +27499,7 @@
         <v>357</v>
       </c>
       <c r="B359" s="7">
-        <v>2025103412</v>
+        <v>2025103385</v>
       </c>
       <c r="C359" s="7">
         <v>1</v>
@@ -27515,10 +27517,10 @@
         <v>250</v>
       </c>
       <c r="H359" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="I359" s="7" t="s">
         <v>900</v>
-      </c>
-      <c r="I359" s="7" t="s">
-        <v>901</v>
       </c>
       <c r="J359" s="7"/>
       <c r="K359" s="7"/>
@@ -27526,13 +27528,13 @@
         <v>245</v>
       </c>
       <c r="M359" s="8" t="s">
+        <v>901</v>
+      </c>
+      <c r="N359" s="8" t="s">
         <v>902</v>
       </c>
-      <c r="N359" s="8" t="s">
-        <v>903</v>
-      </c>
       <c r="O359" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P359" s="7"/>
       <c r="Q359" s="7"/>
@@ -27549,7 +27551,7 @@
       <c r="X359" s="7"/>
       <c r="Y359" s="7"/>
       <c r="Z359" s="8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="AA359" s="7" t="s">
         <v>40</v>
@@ -27563,7 +27565,7 @@
         <v>358</v>
       </c>
       <c r="B360" s="3">
-        <v>2025103385</v>
+        <v>2025103297</v>
       </c>
       <c r="C360" s="3">
         <v>1</v>
@@ -27581,33 +27583,35 @@
         <v>250</v>
       </c>
       <c r="H360" s="3" t="s">
-        <v>383</v>
+        <v>903</v>
       </c>
       <c r="I360" s="3" t="s">
-        <v>901</v>
-      </c>
-      <c r="J360" s="3"/>
-      <c r="K360" s="3"/>
+        <v>900</v>
+      </c>
+      <c r="J360" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="K360" s="3" t="s">
+        <v>263</v>
+      </c>
       <c r="L360" s="6" t="s">
         <v>245</v>
       </c>
       <c r="M360" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="N360" s="6" t="s">
         <v>902</v>
       </c>
-      <c r="N360" s="6" t="s">
-        <v>903</v>
-      </c>
       <c r="O360" s="3" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="P360" s="3"/>
       <c r="Q360" s="3"/>
       <c r="R360" s="3">
         <v>0</v>
       </c>
-      <c r="S360" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S360" s="3"/>
       <c r="T360" s="3"/>
       <c r="U360" s="3"/>
       <c r="V360" s="3"/>
@@ -27615,7 +27619,7 @@
       <c r="X360" s="3"/>
       <c r="Y360" s="3"/>
       <c r="Z360" s="6" t="s">
-        <v>248</v>
+        <v>904</v>
       </c>
       <c r="AA360" s="3" t="s">
         <v>40</v>
@@ -27645,10 +27649,10 @@
         <v>250</v>
       </c>
       <c r="H361" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="I361" s="7" t="s">
         <v>900</v>
-      </c>
-      <c r="I361" s="7" t="s">
-        <v>901</v>
       </c>
       <c r="J361" s="7"/>
       <c r="K361" s="7"/>
@@ -27656,13 +27660,13 @@
         <v>245</v>
       </c>
       <c r="M361" s="8" t="s">
+        <v>901</v>
+      </c>
+      <c r="N361" s="8" t="s">
         <v>902</v>
       </c>
-      <c r="N361" s="8" t="s">
-        <v>903</v>
-      </c>
       <c r="O361" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P361" s="7"/>
       <c r="Q361" s="7"/>
@@ -27679,7 +27683,7 @@
       <c r="X361" s="7"/>
       <c r="Y361" s="7"/>
       <c r="Z361" s="8" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="AA361" s="7" t="s">
         <v>40</v>
@@ -27691,7 +27695,7 @@
         <v>360</v>
       </c>
       <c r="B362" s="3">
-        <v>2025103297</v>
+        <v>2025103412</v>
       </c>
       <c r="C362" s="3">
         <v>1</v>
@@ -27709,35 +27713,33 @@
         <v>250</v>
       </c>
       <c r="H362" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="I362" s="3" t="s">
         <v>900</v>
       </c>
-      <c r="I362" s="3" t="s">
-        <v>901</v>
-      </c>
-      <c r="J362" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="K362" s="3" t="s">
-        <v>263</v>
-      </c>
+      <c r="J362" s="3"/>
+      <c r="K362" s="3"/>
       <c r="L362" s="6" t="s">
         <v>245</v>
       </c>
       <c r="M362" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="N362" s="6" t="s">
         <v>902</v>
       </c>
-      <c r="N362" s="6" t="s">
-        <v>903</v>
-      </c>
       <c r="O362" s="3" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="P362" s="3"/>
       <c r="Q362" s="3"/>
       <c r="R362" s="3">
         <v>0</v>
       </c>
-      <c r="S362" s="3"/>
+      <c r="S362" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T362" s="3"/>
       <c r="U362" s="3"/>
       <c r="V362" s="3"/>
@@ -27745,7 +27747,7 @@
       <c r="X362" s="3"/>
       <c r="Y362" s="3"/>
       <c r="Z362" s="6" t="s">
-        <v>905</v>
+        <v>255</v>
       </c>
       <c r="AA362" s="3" t="s">
         <v>40</v>
@@ -27919,7 +27921,7 @@
         <v>916</v>
       </c>
       <c r="AB365" s="9">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>